<commit_message>
added missing coordinates to M25
</commit_message>
<xml_diff>
--- a/Pit_Output/2017-02-07/PIT_M22/pit_20170207_M22.xlsx
+++ b/Pit_Output/2017-02-07/PIT_M22/pit_20170207_M22.xlsx
@@ -2415,7 +2415,7 @@
   <dimension ref="A1:AMK33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:L2"/>
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7621,7 +7621,10 @@
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
-      <c r="F6" s="33"/>
+      <c r="F6" s="33">
+        <f>173</f>
+        <v>173</v>
+      </c>
       <c r="G6" s="33"/>
       <c r="H6" s="32" t="s">
         <v>17</v>

</xml_diff>